<commit_message>
:wrench: | Cosmo search and display items
</commit_message>
<xml_diff>
--- a/cosmo/data/xlsx/data.xlsx
+++ b/cosmo/data/xlsx/data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus\projects\judite\judite\data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus\projects\python\cosmo\cosmo\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E77AAC-F813-4CFF-B2B9-EC45CD9189DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD91F541-D30F-49A9-9056-8F0613B54798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DC77D82C-3D1A-4928-B2F9-AAED9DFD6818}"/>
   </bookViews>
   <sheets>
     <sheet name="livros" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nome</t>
   </si>
@@ -42,13 +41,55 @@
     <t>Edicao</t>
   </si>
   <si>
-    <t>Batata1</t>
-  </si>
-  <si>
-    <t>Batata2</t>
-  </si>
-  <si>
-    <t>Batata3</t>
+    <t>Don Quixote</t>
+  </si>
+  <si>
+    <t>Um Conto de Duas Cidades</t>
+  </si>
+  <si>
+    <t>O Senhor dos Anéis</t>
+  </si>
+  <si>
+    <t>O Pequeno Príncipe</t>
+  </si>
+  <si>
+    <t>Harry Potter e a Pedra Filosofal</t>
+  </si>
+  <si>
+    <t>O Hobbit</t>
+  </si>
+  <si>
+    <t>O Caso dos Dez Negrinhos</t>
+  </si>
+  <si>
+    <t>O Sonho da Câmara Vermelha</t>
+  </si>
+  <si>
+    <t>Ela, a Feiticeira</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Miguel de Cervantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Charles Dickens</t>
+  </si>
+  <si>
+    <t>J. R. R. Tolkien</t>
+  </si>
+  <si>
+    <t>Antoine de Saint-Exupéry</t>
+  </si>
+  <si>
+    <t>J. K. Rowling</t>
+  </si>
+  <si>
+    <t>Agatha Christie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cao Xueqin</t>
   </si>
 </sst>
 </file>
@@ -401,48 +442,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D572D7D-88C3-4819-9C50-871D6BFF0109}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>